<commit_message>
Created TC2 - InvalidLogin
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
     <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="InvalidLogin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>pointofsale</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -408,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,12 +447,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>